<commit_message>
Sprint plan and more
</commit_message>
<xml_diff>
--- a/Research Proposal/Sprint Plan - Anish .xlsx
+++ b/Research Proposal/Sprint Plan - Anish .xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\Masters\MSc in Data Science\Research Proposal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D9ECA5C8-6E65-4E04-A7F9-3DF411878942}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{68E061FD-67F1-458E-BD86-E43145DFC704}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4080" yWindow="0" windowWidth="19470" windowHeight="8130" xr2:uid="{2FF2F005-B7A1-459F-86C9-E4256973273A}"/>
+    <workbookView xWindow="5100" yWindow="0" windowWidth="19470" windowHeight="8130" activeTab="1" xr2:uid="{2FF2F005-B7A1-459F-86C9-E4256973273A}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Timeline" sheetId="3" r:id="rId1"/>
-    <sheet name="HR MVP 3.0 Timeline v1" sheetId="1" state="hidden" r:id="rId2"/>
-    <sheet name="Shortlisted Metrics - Next Step" sheetId="2" state="hidden" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId2"/>
+    <sheet name="HR MVP 3.0 Timeline v1" sheetId="1" state="hidden" r:id="rId3"/>
+    <sheet name="Shortlisted Metrics - Next Step" sheetId="2" state="hidden" r:id="rId4"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="153">
   <si>
     <t xml:space="preserve">HR Analytics - MVP 3.0 Gantt Chart </t>
   </si>
@@ -499,6 +500,45 @@
   </si>
   <si>
     <t>Finish work on final presentation</t>
+  </si>
+  <si>
+    <t>Project Phase</t>
+  </si>
+  <si>
+    <t>Contingency Plan</t>
+  </si>
+  <si>
+    <t>Risk</t>
+  </si>
+  <si>
+    <t>Data Transformation</t>
+  </si>
+  <si>
+    <t>Model Building</t>
+  </si>
+  <si>
+    <t>Did not receive accurate data and the data is corrupted</t>
+  </si>
+  <si>
+    <t>Leverage a copy of the data stored on Google Drive for the same</t>
+  </si>
+  <si>
+    <t>Use a online iPython service like Google Colab to perform the study</t>
+  </si>
+  <si>
+    <t>Data transformation is time consuming and does not result in the format</t>
+  </si>
+  <si>
+    <t>Revisit the exploratory data analysis phase and try alternate methods</t>
+  </si>
+  <si>
+    <t>Might not be able to implement all of the modeling techniques researched during the research space</t>
+  </si>
+  <si>
+    <t>Scale back by filtering modeling techniques prioritized on novelty and usage</t>
+  </si>
+  <si>
+    <t>Jupyter Notebook on the local computer is corrupted</t>
   </si>
 </sst>
 </file>
@@ -1151,7 +1191,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1349,18 +1389,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1377,6 +1405,27 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3528,8 +3577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB4CCD88-19C0-4D30-AF9A-5D44D920AF68}">
   <dimension ref="B1:Y1048527"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView showGridLines="0" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3550,39 +3599,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B1" s="104"/>
-      <c r="C1" s="104"/>
+      <c r="B1" s="100"/>
+      <c r="C1" s="100"/>
     </row>
     <row r="2" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B2" s="105" t="s">
+      <c r="B2" s="101" t="s">
         <v>117</v>
       </c>
-      <c r="C2" s="105"/>
-      <c r="D2" s="105"/>
-      <c r="E2" s="105"/>
-      <c r="F2" s="105"/>
-      <c r="G2" s="105"/>
-      <c r="H2" s="105"/>
-      <c r="I2" s="105"/>
-      <c r="J2" s="105"/>
-      <c r="K2" s="105"/>
-      <c r="L2" s="105"/>
-      <c r="M2" s="105"/>
-      <c r="N2" s="105"/>
-      <c r="O2" s="105"/>
-      <c r="P2" s="105"/>
-      <c r="Q2" s="105"/>
-      <c r="R2" s="105"/>
-      <c r="S2" s="105"/>
-      <c r="T2" s="105"/>
-      <c r="U2" s="105"/>
-      <c r="V2" s="105"/>
-      <c r="W2" s="105"/>
-      <c r="X2" s="105"/>
-      <c r="Y2" s="105"/>
+      <c r="C2" s="101"/>
+      <c r="D2" s="101"/>
+      <c r="E2" s="101"/>
+      <c r="F2" s="101"/>
+      <c r="G2" s="101"/>
+      <c r="H2" s="101"/>
+      <c r="I2" s="101"/>
+      <c r="J2" s="101"/>
+      <c r="K2" s="101"/>
+      <c r="L2" s="101"/>
+      <c r="M2" s="101"/>
+      <c r="N2" s="101"/>
+      <c r="O2" s="101"/>
+      <c r="P2" s="101"/>
+      <c r="Q2" s="101"/>
+      <c r="R2" s="101"/>
+      <c r="S2" s="101"/>
+      <c r="T2" s="101"/>
+      <c r="U2" s="101"/>
+      <c r="V2" s="101"/>
+      <c r="W2" s="101"/>
+      <c r="X2" s="101"/>
+      <c r="Y2" s="101"/>
     </row>
     <row r="3" spans="2:25" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="99"/>
+      <c r="B3" s="95"/>
       <c r="C3" s="91" t="s">
         <v>94</v>
       </c>
@@ -3654,7 +3703,7 @@
       </c>
     </row>
     <row r="4" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B4" s="100" t="s">
+      <c r="B4" s="96" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="93" t="s">
@@ -3731,8 +3780,8 @@
       <c r="B5" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="C5" s="103"/>
-      <c r="D5" s="103"/>
+      <c r="C5" s="99"/>
+      <c r="D5" s="99"/>
       <c r="E5" s="17"/>
       <c r="F5" s="11"/>
       <c r="G5" s="11"/>
@@ -3774,7 +3823,7 @@
         <v>119</v>
       </c>
       <c r="C6" s="17"/>
-      <c r="D6" s="103"/>
+      <c r="D6" s="99"/>
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
       <c r="G6" s="11"/>
@@ -3802,9 +3851,9 @@
         <v>120</v>
       </c>
       <c r="C7" s="17"/>
-      <c r="D7" s="103"/>
-      <c r="E7" s="103"/>
-      <c r="F7" s="103"/>
+      <c r="D7" s="99"/>
+      <c r="E7" s="99"/>
+      <c r="F7" s="99"/>
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
       <c r="I7" s="11"/>
@@ -3830,9 +3879,9 @@
         <v>122</v>
       </c>
       <c r="C8" s="17"/>
-      <c r="D8" s="103"/>
-      <c r="E8" s="103"/>
-      <c r="F8" s="103"/>
+      <c r="D8" s="99"/>
+      <c r="E8" s="99"/>
+      <c r="F8" s="99"/>
       <c r="G8" s="11"/>
       <c r="H8" s="11"/>
       <c r="I8" s="11"/>
@@ -3854,14 +3903,14 @@
       <c r="Y8" s="11"/>
     </row>
     <row r="9" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B9" s="101" t="s">
+      <c r="B9" s="97" t="s">
         <v>121</v>
       </c>
-      <c r="C9" s="101"/>
-      <c r="D9" s="101"/>
-      <c r="E9" s="101"/>
-      <c r="F9" s="103"/>
-      <c r="G9" s="103"/>
+      <c r="C9" s="97"/>
+      <c r="D9" s="97"/>
+      <c r="E9" s="97"/>
+      <c r="F9" s="99"/>
+      <c r="G9" s="99"/>
       <c r="H9" s="11"/>
       <c r="I9" s="11"/>
       <c r="J9" s="11"/>
@@ -3882,15 +3931,15 @@
       <c r="Y9" s="11"/>
     </row>
     <row r="10" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B10" s="102" t="s">
+      <c r="B10" s="98" t="s">
         <v>123</v>
       </c>
       <c r="C10" s="17"/>
       <c r="D10" s="17"/>
       <c r="E10" s="17"/>
       <c r="F10" s="11"/>
-      <c r="G10" s="103"/>
-      <c r="H10" s="103"/>
+      <c r="G10" s="99"/>
+      <c r="H10" s="99"/>
       <c r="I10" s="11"/>
       <c r="J10" s="11"/>
       <c r="K10" s="11"/>
@@ -3918,8 +3967,8 @@
       <c r="E11" s="17"/>
       <c r="F11" s="11"/>
       <c r="G11" s="11"/>
-      <c r="H11" s="103"/>
-      <c r="I11" s="103"/>
+      <c r="H11" s="99"/>
+      <c r="I11" s="99"/>
       <c r="J11" s="11"/>
       <c r="K11" s="11"/>
       <c r="L11" s="11"/>
@@ -3946,8 +3995,8 @@
       <c r="E12" s="17"/>
       <c r="F12" s="11"/>
       <c r="G12" s="11"/>
-      <c r="H12" s="103"/>
-      <c r="I12" s="103"/>
+      <c r="H12" s="99"/>
+      <c r="I12" s="99"/>
       <c r="J12" s="11"/>
       <c r="K12" s="11"/>
       <c r="L12" s="11"/>
@@ -3974,8 +4023,8 @@
       <c r="E13" s="17"/>
       <c r="F13" s="11"/>
       <c r="G13" s="11"/>
-      <c r="H13" s="103"/>
-      <c r="I13" s="103"/>
+      <c r="H13" s="99"/>
+      <c r="I13" s="99"/>
       <c r="J13" s="11"/>
       <c r="K13" s="11"/>
       <c r="L13" s="11"/>
@@ -4003,8 +4052,8 @@
       <c r="F14" s="11"/>
       <c r="G14" s="11"/>
       <c r="H14" s="11"/>
-      <c r="I14" s="103"/>
-      <c r="J14" s="103"/>
+      <c r="I14" s="99"/>
+      <c r="J14" s="99"/>
       <c r="K14" s="17"/>
       <c r="L14" s="11"/>
       <c r="M14" s="17"/>
@@ -4031,8 +4080,8 @@
       <c r="F15" s="11"/>
       <c r="G15" s="11"/>
       <c r="H15" s="11"/>
-      <c r="I15" s="103"/>
-      <c r="J15" s="103"/>
+      <c r="I15" s="99"/>
+      <c r="J15" s="99"/>
       <c r="K15" s="17"/>
       <c r="L15" s="11"/>
       <c r="M15" s="17"/>
@@ -4050,18 +4099,18 @@
       <c r="Y15" s="17"/>
     </row>
     <row r="16" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B16" s="101" t="s">
+      <c r="B16" s="97" t="s">
         <v>129</v>
       </c>
-      <c r="C16" s="101"/>
-      <c r="D16" s="101"/>
-      <c r="E16" s="101"/>
-      <c r="F16" s="101"/>
-      <c r="G16" s="101"/>
-      <c r="H16" s="101"/>
-      <c r="I16" s="101"/>
-      <c r="J16" s="103"/>
-      <c r="K16" s="103"/>
+      <c r="C16" s="97"/>
+      <c r="D16" s="97"/>
+      <c r="E16" s="97"/>
+      <c r="F16" s="97"/>
+      <c r="G16" s="97"/>
+      <c r="H16" s="97"/>
+      <c r="I16" s="97"/>
+      <c r="J16" s="99"/>
+      <c r="K16" s="99"/>
       <c r="L16" s="11"/>
       <c r="M16" s="17"/>
       <c r="N16" s="11"/>
@@ -4078,7 +4127,7 @@
       <c r="Y16" s="17"/>
     </row>
     <row r="17" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B17" s="102" t="s">
+      <c r="B17" s="98" t="s">
         <v>130</v>
       </c>
       <c r="C17" s="17"/>
@@ -4089,8 +4138,8 @@
       <c r="H17" s="11"/>
       <c r="I17" s="11"/>
       <c r="J17" s="11"/>
-      <c r="K17" s="103"/>
-      <c r="L17" s="103"/>
+      <c r="K17" s="99"/>
+      <c r="L17" s="99"/>
       <c r="M17" s="17"/>
       <c r="N17" s="11"/>
       <c r="O17" s="17"/>
@@ -4118,11 +4167,11 @@
       <c r="I18" s="11"/>
       <c r="J18" s="11"/>
       <c r="K18" s="17"/>
-      <c r="L18" s="103"/>
-      <c r="M18" s="103"/>
-      <c r="N18" s="103"/>
-      <c r="O18" s="103"/>
-      <c r="P18" s="103"/>
+      <c r="L18" s="99"/>
+      <c r="M18" s="99"/>
+      <c r="N18" s="99"/>
+      <c r="O18" s="99"/>
+      <c r="P18" s="99"/>
       <c r="Q18" s="17"/>
       <c r="R18" s="11"/>
       <c r="S18" s="17"/>
@@ -4148,10 +4197,10 @@
       <c r="K19" s="17"/>
       <c r="L19" s="11"/>
       <c r="M19" s="17"/>
-      <c r="N19" s="103"/>
-      <c r="O19" s="103"/>
-      <c r="P19" s="103"/>
-      <c r="Q19" s="103"/>
+      <c r="N19" s="99"/>
+      <c r="O19" s="99"/>
+      <c r="P19" s="99"/>
+      <c r="Q19" s="99"/>
       <c r="R19" s="11"/>
       <c r="S19" s="17"/>
       <c r="T19" s="11"/>
@@ -4178,9 +4227,9 @@
       <c r="M20" s="17"/>
       <c r="N20" s="11"/>
       <c r="O20" s="11"/>
-      <c r="P20" s="103"/>
-      <c r="Q20" s="103"/>
-      <c r="R20" s="103"/>
+      <c r="P20" s="99"/>
+      <c r="Q20" s="99"/>
+      <c r="R20" s="99"/>
       <c r="S20" s="17"/>
       <c r="T20" s="11"/>
       <c r="U20" s="17"/>
@@ -4206,9 +4255,9 @@
       <c r="M21" s="11"/>
       <c r="N21" s="11"/>
       <c r="O21" s="11"/>
-      <c r="P21" s="103"/>
-      <c r="Q21" s="103"/>
-      <c r="R21" s="103"/>
+      <c r="P21" s="99"/>
+      <c r="Q21" s="99"/>
+      <c r="R21" s="99"/>
       <c r="S21" s="11"/>
       <c r="T21" s="11"/>
       <c r="U21" s="11"/>
@@ -4235,9 +4284,9 @@
       <c r="N22" s="11"/>
       <c r="O22" s="11"/>
       <c r="P22" s="11"/>
-      <c r="Q22" s="103"/>
-      <c r="R22" s="103"/>
-      <c r="S22" s="103"/>
+      <c r="Q22" s="99"/>
+      <c r="R22" s="99"/>
+      <c r="S22" s="99"/>
       <c r="T22" s="11"/>
       <c r="U22" s="11"/>
       <c r="V22" s="11"/>
@@ -4265,10 +4314,10 @@
       <c r="P23" s="11"/>
       <c r="Q23" s="11"/>
       <c r="R23" s="11"/>
-      <c r="S23" s="103"/>
-      <c r="T23" s="103"/>
-      <c r="U23" s="103"/>
-      <c r="V23" s="103"/>
+      <c r="S23" s="99"/>
+      <c r="T23" s="99"/>
+      <c r="U23" s="99"/>
+      <c r="V23" s="99"/>
       <c r="W23" s="11"/>
       <c r="X23" s="11"/>
       <c r="Y23" s="11"/>
@@ -4296,13 +4345,13 @@
       <c r="S24" s="11"/>
       <c r="T24" s="11"/>
       <c r="U24" s="11"/>
-      <c r="V24" s="103"/>
-      <c r="W24" s="103"/>
+      <c r="V24" s="99"/>
+      <c r="W24" s="99"/>
       <c r="X24" s="11"/>
       <c r="Y24" s="11"/>
     </row>
     <row r="25" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B25" s="102" t="s">
+      <c r="B25" s="98" t="s">
         <v>138</v>
       </c>
       <c r="C25" s="17"/>
@@ -4325,37 +4374,37 @@
       <c r="T25" s="11"/>
       <c r="U25" s="17"/>
       <c r="V25" s="11"/>
-      <c r="W25" s="103"/>
-      <c r="X25" s="103"/>
+      <c r="W25" s="99"/>
+      <c r="X25" s="99"/>
       <c r="Y25" s="17"/>
     </row>
     <row r="26" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B26" s="101" t="s">
+      <c r="B26" s="97" t="s">
         <v>139</v>
       </c>
-      <c r="C26" s="101"/>
-      <c r="D26" s="101"/>
-      <c r="E26" s="101"/>
-      <c r="F26" s="101"/>
-      <c r="G26" s="101"/>
-      <c r="H26" s="101"/>
-      <c r="I26" s="101"/>
-      <c r="J26" s="101"/>
-      <c r="K26" s="101"/>
-      <c r="L26" s="101"/>
-      <c r="M26" s="101"/>
-      <c r="N26" s="101"/>
-      <c r="O26" s="101"/>
-      <c r="P26" s="101"/>
-      <c r="Q26" s="101"/>
-      <c r="R26" s="101"/>
-      <c r="S26" s="101"/>
-      <c r="T26" s="101"/>
-      <c r="U26" s="101"/>
-      <c r="V26" s="101"/>
-      <c r="W26" s="101"/>
-      <c r="X26" s="103"/>
-      <c r="Y26" s="103"/>
+      <c r="C26" s="97"/>
+      <c r="D26" s="97"/>
+      <c r="E26" s="97"/>
+      <c r="F26" s="97"/>
+      <c r="G26" s="97"/>
+      <c r="H26" s="97"/>
+      <c r="I26" s="97"/>
+      <c r="J26" s="97"/>
+      <c r="K26" s="97"/>
+      <c r="L26" s="97"/>
+      <c r="M26" s="97"/>
+      <c r="N26" s="97"/>
+      <c r="O26" s="97"/>
+      <c r="P26" s="97"/>
+      <c r="Q26" s="97"/>
+      <c r="R26" s="97"/>
+      <c r="S26" s="97"/>
+      <c r="T26" s="97"/>
+      <c r="U26" s="97"/>
+      <c r="V26" s="97"/>
+      <c r="W26" s="97"/>
+      <c r="X26" s="99"/>
+      <c r="Y26" s="99"/>
     </row>
     <row r="27" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B27" s="46"/>
@@ -4386,6 +4435,84 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{736C7757-70E8-446A-966C-65AF1A56E60B}">
+  <dimension ref="B2:D7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="96" t="s">
+        <v>140</v>
+      </c>
+      <c r="C2" s="96" t="s">
+        <v>142</v>
+      </c>
+      <c r="D2" s="96" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="107" t="s">
+        <v>124</v>
+      </c>
+      <c r="C3" s="107" t="s">
+        <v>145</v>
+      </c>
+      <c r="D3" s="107" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="108" t="s">
+        <v>143</v>
+      </c>
+      <c r="C4" s="107" t="s">
+        <v>152</v>
+      </c>
+      <c r="D4" s="107" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="108"/>
+      <c r="C5" s="107" t="s">
+        <v>148</v>
+      </c>
+      <c r="D5" s="107" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="98" t="s">
+        <v>144</v>
+      </c>
+      <c r="C6" s="107" t="s">
+        <v>150</v>
+      </c>
+      <c r="D6" s="107" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="106"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B4:B5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{485E0184-C785-415D-8448-F2CFB2DFCBA2}">
   <dimension ref="A1:L42"/>
   <sheetViews>
@@ -4450,26 +4577,26 @@
       <c r="B4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="95" t="s">
+      <c r="C4" s="102" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="96"/>
-      <c r="E4" s="97"/>
-      <c r="F4" s="95" t="s">
+      <c r="D4" s="103"/>
+      <c r="E4" s="104"/>
+      <c r="F4" s="102" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="97"/>
-      <c r="H4" s="95" t="s">
+      <c r="G4" s="104"/>
+      <c r="H4" s="102" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="97"/>
+      <c r="I4" s="104"/>
       <c r="J4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="K4" s="95" t="s">
+      <c r="K4" s="102" t="s">
         <v>15</v>
       </c>
-      <c r="L4" s="98"/>
+      <c r="L4" s="105"/>
     </row>
     <row r="5" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="7" t="s">
@@ -5010,7 +5137,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A807533-DF42-484A-9AAD-6CADD51D41BB}">
   <dimension ref="A1:E4"/>
   <sheetViews>
@@ -5094,12 +5221,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5275,15 +5399,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E8B4D14F-B555-4BB7-B3D8-341CBA30C9B5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{216E3C58-1D32-4DDF-83D5-37D00941E9CD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="0de0b368-6c25-428c-a548-77fa2d528b83"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5307,17 +5442,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{216E3C58-1D32-4DDF-83D5-37D00941E9CD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E8B4D14F-B555-4BB7-B3D8-341CBA30C9B5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="0de0b368-6c25-428c-a548-77fa2d528b83"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>